<commit_message>
All peeps in garden 🙌🦄
</commit_message>
<xml_diff>
--- a/Garden App/Peeps Accounting.xlsx
+++ b/Garden App/Peeps Accounting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lars-\source\repos\open source\cg2020-group-picture-another-dimension\Garden App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35F8CCF2-C4AA-4984-8375-AA82EA10268A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50061B83-6A6E-4822-846E-838E186FCBF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38880" yWindow="60" windowWidth="17055" windowHeight="15600" xr2:uid="{8684E3AA-EC06-48A7-BFAE-7CCFBD7EFAE6}"/>
+    <workbookView xWindow="29190" yWindow="390" windowWidth="17055" windowHeight="15600" xr2:uid="{8684E3AA-EC06-48A7-BFAE-7CCFBD7EFAE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -308,13 +308,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{91054EBE-4800-4CD4-9A7C-F2794396E173}" name="Table1" displayName="Table1" ref="A1:I51" totalsRowShown="0">
-  <autoFilter ref="A1:I51" xr:uid="{1D6FD3FD-DD4E-4958-8C16-1C6223DC65F8}">
-    <filterColumn colId="7">
-      <filters>
-        <filter val="TRUE"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:I51" xr:uid="{1D6FD3FD-DD4E-4958-8C16-1C6223DC65F8}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{F70AE9DF-F9FB-486D-8564-B7D56E3818A4}" name="Name"/>
     <tableColumn id="9" xr3:uid="{7799C646-F115-4391-AD0A-F12801AF397D}" name="No. of peeps"/>
@@ -629,8 +623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D97C0BEB-74C8-4333-889B-395318AF70D1}">
   <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,7 +668,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -700,7 +694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -726,7 +720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -752,7 +746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -778,7 +772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -862,7 +856,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -908,16 +902,16 @@
         <v>0</v>
       </c>
       <c r="G10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -943,7 +937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>68</v>
       </c>
@@ -969,7 +963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>69</v>
       </c>
@@ -995,7 +989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -1021,7 +1015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -1047,7 +1041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -1073,7 +1067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -1119,13 +1113,13 @@
         <v>0</v>
       </c>
       <c r="G18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -1151,7 +1145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -1200,16 +1194,16 @@
         <v>1</v>
       </c>
       <c r="G21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I21" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -1255,13 +1249,13 @@
         <v>1</v>
       </c>
       <c r="G23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -1290,7 +1284,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>38</v>
       </c>
@@ -1316,7 +1310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>39</v>
       </c>
@@ -1342,7 +1336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>40</v>
       </c>
@@ -1368,7 +1362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>41</v>
       </c>
@@ -1394,7 +1388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>66</v>
       </c>
@@ -1440,10 +1434,10 @@
         <v>1</v>
       </c>
       <c r="G30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -1466,10 +1460,10 @@
         <v>0</v>
       </c>
       <c r="G31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I31" t="s">
         <v>44</v>
@@ -1495,10 +1489,10 @@
         <v>0</v>
       </c>
       <c r="G32" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -1521,10 +1515,10 @@
         <v>0</v>
       </c>
       <c r="G33" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -1547,10 +1541,10 @@
         <v>1</v>
       </c>
       <c r="G34" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H34" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -1573,10 +1567,10 @@
         <v>0</v>
       </c>
       <c r="G35" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H35" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -1599,13 +1593,13 @@
         <v>1</v>
       </c>
       <c r="G36" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H36" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>50</v>
       </c>
@@ -1631,7 +1625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>51</v>
       </c>
@@ -1657,7 +1651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>52</v>
       </c>
@@ -1683,7 +1677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>53</v>
       </c>
@@ -1709,7 +1703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>54</v>
       </c>
@@ -1755,10 +1749,10 @@
         <v>0</v>
       </c>
       <c r="G42" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H42" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -1781,13 +1775,13 @@
         <v>0</v>
       </c>
       <c r="G43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H43" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>57</v>
       </c>
@@ -1816,7 +1810,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>59</v>
       </c>
@@ -1845,7 +1839,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>61</v>
       </c>
@@ -1874,7 +1868,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>62</v>
       </c>
@@ -1903,7 +1897,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>63</v>
       </c>
@@ -1932,7 +1926,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>64</v>
       </c>
@@ -1961,7 +1955,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="50" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>70</v>
       </c>
@@ -1987,7 +1981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>71</v>
       </c>

</xml_diff>

<commit_message>
History of the photo
Placed new full size peeps
</commit_message>
<xml_diff>
--- a/Garden App/Peeps Accounting.xlsx
+++ b/Garden App/Peeps Accounting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lars-\source\repos\open source\cg2020-group-picture-another-dimension\Garden App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50061B83-6A6E-4822-846E-838E186FCBF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75382CD5-1270-4974-B94E-ECBA50B5B50A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29190" yWindow="390" windowWidth="17055" windowHeight="15600" xr2:uid="{8684E3AA-EC06-48A7-BFAE-7CCFBD7EFAE6}"/>
+    <workbookView xWindow="38880" yWindow="0" windowWidth="17055" windowHeight="15600" xr2:uid="{8684E3AA-EC06-48A7-BFAE-7CCFBD7EFAE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="77">
   <si>
     <t>Name</t>
   </si>
@@ -252,6 +252,18 @@
   </si>
   <si>
     <t>Michael L.</t>
+  </si>
+  <si>
+    <t>Alan</t>
+  </si>
+  <si>
+    <t>John R.</t>
+  </si>
+  <si>
+    <t>Kris</t>
+  </si>
+  <si>
+    <t>Matt &amp; Lucy w/Lee</t>
   </si>
 </sst>
 </file>
@@ -307,8 +319,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{91054EBE-4800-4CD4-9A7C-F2794396E173}" name="Table1" displayName="Table1" ref="A1:I51" totalsRowShown="0">
-  <autoFilter ref="A1:I51" xr:uid="{1D6FD3FD-DD4E-4958-8C16-1C6223DC65F8}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{91054EBE-4800-4CD4-9A7C-F2794396E173}" name="Table1" displayName="Table1" ref="A1:I55" totalsRowShown="0">
+  <autoFilter ref="A1:I55" xr:uid="{1D6FD3FD-DD4E-4958-8C16-1C6223DC65F8}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{F70AE9DF-F9FB-486D-8564-B7D56E3818A4}" name="Name"/>
     <tableColumn id="9" xr3:uid="{7799C646-F115-4391-AD0A-F12801AF397D}" name="No. of peeps"/>
@@ -621,10 +633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D97C0BEB-74C8-4333-889B-395318AF70D1}">
-  <dimension ref="A1:I51"/>
+  <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H54" sqref="H54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2007,6 +2019,110 @@
         <v>0</v>
       </c>
     </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>73</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52" t="s">
+        <v>28</v>
+      </c>
+      <c r="D52" t="b">
+        <v>1</v>
+      </c>
+      <c r="E52" t="b">
+        <v>1</v>
+      </c>
+      <c r="F52" t="b">
+        <v>0</v>
+      </c>
+      <c r="G52" t="b">
+        <v>1</v>
+      </c>
+      <c r="H52" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>74</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53" t="s">
+        <v>21</v>
+      </c>
+      <c r="D53" t="b">
+        <v>1</v>
+      </c>
+      <c r="E53" t="b">
+        <v>0</v>
+      </c>
+      <c r="F53" t="b">
+        <v>0</v>
+      </c>
+      <c r="G53" t="b">
+        <v>0</v>
+      </c>
+      <c r="H53" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>75</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54" t="s">
+        <v>25</v>
+      </c>
+      <c r="D54" t="b">
+        <v>1</v>
+      </c>
+      <c r="E54" t="b">
+        <v>1</v>
+      </c>
+      <c r="F54" t="b">
+        <v>0</v>
+      </c>
+      <c r="G54" t="b">
+        <v>1</v>
+      </c>
+      <c r="H54" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>76</v>
+      </c>
+      <c r="B55">
+        <v>2</v>
+      </c>
+      <c r="C55" t="s">
+        <v>23</v>
+      </c>
+      <c r="D55" t="b">
+        <v>1</v>
+      </c>
+      <c r="E55" t="b">
+        <v>1</v>
+      </c>
+      <c r="F55" t="b">
+        <v>0</v>
+      </c>
+      <c r="G55" t="b">
+        <v>1</v>
+      </c>
+      <c r="H55" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Anders + Kim & Rune fixed
</commit_message>
<xml_diff>
--- a/Garden App/Peeps Accounting.xlsx
+++ b/Garden App/Peeps Accounting.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lars-\source\repos\open source\cg2020-group-picture-another-dimension\Garden App\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bi-lea\Source\Repos\OpenSource\codegarden-2020-group-image-another-dimension\Garden App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD7373F0-57AA-47AD-8079-C40BEA704808}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{008BE434-FC7A-4B74-A6C8-6207949516FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39225" yWindow="0" windowWidth="17055" windowHeight="15600" xr2:uid="{8684E3AA-EC06-48A7-BFAE-7CCFBD7EFAE6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{8684E3AA-EC06-48A7-BFAE-7CCFBD7EFAE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="79">
   <si>
     <t>Name</t>
   </si>
@@ -80,18 +80,12 @@
     <t>Comment</t>
   </si>
   <si>
-    <t>Doesn't show up in ThreeJS</t>
-  </si>
-  <si>
     <t>Rune</t>
   </si>
   <si>
     <t>Per</t>
   </si>
   <si>
-    <t>Combine with Tombstone in garden</t>
-  </si>
-  <si>
     <t>In garden</t>
   </si>
   <si>
@@ -146,9 +140,6 @@
     <t>Lars</t>
   </si>
   <si>
-    <t>Could do with current picture. 🤪</t>
-  </si>
-  <si>
     <t>Ravi</t>
   </si>
   <si>
@@ -267,6 +258,18 @@
   </si>
   <si>
     <t>Rasmus 2</t>
+  </si>
+  <si>
+    <t>Doug</t>
+  </si>
+  <si>
+    <t>Simone</t>
+  </si>
+  <si>
+    <t>Andrew B.</t>
+  </si>
+  <si>
+    <t>Nick W.</t>
   </si>
 </sst>
 </file>
@@ -322,8 +325,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{91054EBE-4800-4CD4-9A7C-F2794396E173}" name="Table1" displayName="Table1" ref="A1:I56" totalsRowShown="0">
-  <autoFilter ref="A1:I56" xr:uid="{1D6FD3FD-DD4E-4958-8C16-1C6223DC65F8}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{91054EBE-4800-4CD4-9A7C-F2794396E173}" name="Table1" displayName="Table1" ref="A1:I60" totalsRowShown="0">
+  <autoFilter ref="A1:I60" xr:uid="{1D6FD3FD-DD4E-4958-8C16-1C6223DC65F8}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{F70AE9DF-F9FB-486D-8564-B7D56E3818A4}" name="Name"/>
     <tableColumn id="9" xr3:uid="{7799C646-F115-4391-AD0A-F12801AF397D}" name="No. of peeps"/>
@@ -636,10 +639,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D97C0BEB-74C8-4333-889B-395318AF70D1}">
-  <dimension ref="A1:I56"/>
+  <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H55" sqref="H55"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -659,7 +662,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -674,7 +677,7 @@
         <v>10</v>
       </c>
       <c r="G1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H1" t="s">
         <v>11</v>
@@ -833,18 +836,15 @@
         <v>0</v>
       </c>
       <c r="G7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" t="b">
-        <v>1</v>
-      </c>
-      <c r="I7" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -862,18 +862,15 @@
         <v>0</v>
       </c>
       <c r="G8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" t="b">
-        <v>1</v>
-      </c>
-      <c r="I8" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -899,13 +896,13 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D10" t="b">
         <v>1</v>
@@ -921,20 +918,17 @@
       </c>
       <c r="H10" t="b">
         <v>0</v>
-      </c>
-      <c r="I10" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D11" t="b">
         <v>1</v>
@@ -954,13 +948,13 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D12" t="b">
         <v>1</v>
@@ -980,13 +974,13 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B13">
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D13" t="b">
         <v>1</v>
@@ -1006,13 +1000,13 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B14">
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D14" t="b">
         <v>1</v>
@@ -1032,13 +1026,13 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D15" t="b">
         <v>1</v>
@@ -1058,13 +1052,13 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B16">
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D16" t="b">
         <v>1</v>
@@ -1084,13 +1078,13 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D17" t="b">
         <v>1</v>
@@ -1110,13 +1104,13 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D18" t="b">
         <v>1</v>
@@ -1136,13 +1130,13 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D19" t="b">
         <v>1</v>
@@ -1162,13 +1156,13 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D20" t="b">
         <v>1</v>
@@ -1186,18 +1180,18 @@
         <v>0</v>
       </c>
       <c r="I20" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D21" t="b">
         <v>1</v>
@@ -1215,18 +1209,18 @@
         <v>0</v>
       </c>
       <c r="I21" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D22" t="b">
         <v>1</v>
@@ -1246,13 +1240,13 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D23" t="b">
         <v>1</v>
@@ -1272,13 +1266,13 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D24" t="b">
         <v>1</v>
@@ -1294,20 +1288,17 @@
       </c>
       <c r="H24" t="b">
         <v>0</v>
-      </c>
-      <c r="I24" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B25">
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D25" t="b">
         <v>1</v>
@@ -1327,13 +1318,13 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D26" t="b">
         <v>1</v>
@@ -1353,13 +1344,13 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D27" t="b">
         <v>1</v>
@@ -1379,13 +1370,13 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B28">
         <v>5</v>
       </c>
       <c r="C28" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D28" t="b">
         <v>1</v>
@@ -1405,13 +1396,13 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D29" t="b">
         <v>1</v>
@@ -1431,13 +1422,13 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B30">
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D30" t="b">
         <v>1</v>
@@ -1457,13 +1448,13 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D31" t="b">
         <v>1</v>
@@ -1481,18 +1472,18 @@
         <v>0</v>
       </c>
       <c r="I31" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D32" t="b">
         <v>1</v>
@@ -1512,13 +1503,13 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B33">
         <v>2</v>
       </c>
       <c r="C33" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D33" t="b">
         <v>1</v>
@@ -1538,13 +1529,13 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D34" t="b">
         <v>1</v>
@@ -1564,13 +1555,13 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D35" t="b">
         <v>1</v>
@@ -1590,13 +1581,13 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D36" t="b">
         <v>1</v>
@@ -1616,7 +1607,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -1642,13 +1633,13 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B38">
         <v>0</v>
       </c>
       <c r="C38" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D38" t="b">
         <v>1</v>
@@ -1668,13 +1659,13 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B39">
         <v>7</v>
       </c>
       <c r="C39" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D39" t="b">
         <v>1</v>
@@ -1694,13 +1685,13 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B40">
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D40" t="b">
         <v>1</v>
@@ -1720,13 +1711,13 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B41">
         <v>2</v>
       </c>
       <c r="C41" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D41" t="b">
         <v>1</v>
@@ -1746,13 +1737,13 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B42">
         <v>1</v>
       </c>
       <c r="C42" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D42" t="b">
         <v>1</v>
@@ -1772,13 +1763,13 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B43">
         <v>1</v>
       </c>
       <c r="C43" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D43" t="b">
         <v>1</v>
@@ -1798,13 +1789,13 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B44">
         <v>0</v>
       </c>
       <c r="C44" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D44" t="b">
         <v>1</v>
@@ -1822,18 +1813,18 @@
         <v>0</v>
       </c>
       <c r="I44" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B45">
         <v>1</v>
       </c>
       <c r="C45" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D45" t="b">
         <v>1</v>
@@ -1851,18 +1842,18 @@
         <v>0</v>
       </c>
       <c r="I45" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B46">
         <v>0</v>
       </c>
       <c r="C46" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D46" t="b">
         <v>1</v>
@@ -1880,18 +1871,18 @@
         <v>0</v>
       </c>
       <c r="I46" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B47">
         <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D47" t="b">
         <v>1</v>
@@ -1909,18 +1900,18 @@
         <v>0</v>
       </c>
       <c r="I47" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B48">
         <v>1</v>
       </c>
       <c r="C48" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D48" t="b">
         <v>1</v>
@@ -1938,18 +1929,18 @@
         <v>0</v>
       </c>
       <c r="I48" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B49">
         <v>1</v>
       </c>
       <c r="C49" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D49" t="b">
         <v>1</v>
@@ -1967,18 +1958,18 @@
         <v>0</v>
       </c>
       <c r="I49" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B50">
         <v>0</v>
       </c>
       <c r="C50" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D50" t="b">
         <v>1</v>
@@ -1998,13 +1989,13 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B51">
         <v>1</v>
       </c>
       <c r="C51" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D51" t="b">
         <v>1</v>
@@ -2024,13 +2015,13 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B52">
         <v>1</v>
       </c>
       <c r="C52" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D52" t="b">
         <v>1</v>
@@ -2050,13 +2041,13 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B53">
         <v>1</v>
       </c>
       <c r="C53" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D53" t="b">
         <v>1</v>
@@ -2076,13 +2067,13 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B54">
         <v>1</v>
       </c>
       <c r="C54" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D54" t="b">
         <v>1</v>
@@ -2102,13 +2093,13 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B55">
         <v>2</v>
       </c>
       <c r="C55" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D55" t="b">
         <v>1</v>
@@ -2128,28 +2119,132 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>74</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="C56" t="s">
+        <v>26</v>
+      </c>
+      <c r="D56" t="b">
+        <v>1</v>
+      </c>
+      <c r="E56" t="b">
+        <v>1</v>
+      </c>
+      <c r="F56" t="b">
+        <v>0</v>
+      </c>
+      <c r="G56" t="b">
+        <v>1</v>
+      </c>
+      <c r="H56" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>75</v>
+      </c>
+      <c r="B57">
+        <v>1</v>
+      </c>
+      <c r="C57" t="s">
+        <v>26</v>
+      </c>
+      <c r="D57" t="b">
+        <v>1</v>
+      </c>
+      <c r="E57" t="b">
+        <v>0</v>
+      </c>
+      <c r="F57" t="b">
+        <v>0</v>
+      </c>
+      <c r="G57" t="b">
+        <v>0</v>
+      </c>
+      <c r="H57" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>76</v>
+      </c>
+      <c r="B58">
+        <v>1</v>
+      </c>
+      <c r="C58" t="s">
+        <v>23</v>
+      </c>
+      <c r="D58" t="b">
+        <v>1</v>
+      </c>
+      <c r="E58" t="b">
+        <v>0</v>
+      </c>
+      <c r="F58" t="b">
+        <v>0</v>
+      </c>
+      <c r="G58" t="b">
+        <v>0</v>
+      </c>
+      <c r="H58" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>77</v>
       </c>
-      <c r="B56">
-        <v>1</v>
-      </c>
-      <c r="C56" t="s">
-        <v>28</v>
-      </c>
-      <c r="D56" t="b">
-        <v>1</v>
-      </c>
-      <c r="E56" t="b">
-        <v>1</v>
-      </c>
-      <c r="F56" t="b">
-        <v>0</v>
-      </c>
-      <c r="G56" t="b">
-        <v>1</v>
-      </c>
-      <c r="H56" t="b">
-        <v>0</v>
+      <c r="B59">
+        <v>1</v>
+      </c>
+      <c r="C59" t="s">
+        <v>19</v>
+      </c>
+      <c r="D59" t="b">
+        <v>1</v>
+      </c>
+      <c r="E59" t="b">
+        <v>0</v>
+      </c>
+      <c r="F59" t="b">
+        <v>0</v>
+      </c>
+      <c r="G59" t="b">
+        <v>0</v>
+      </c>
+      <c r="H59" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>78</v>
+      </c>
+      <c r="B60">
+        <v>1</v>
+      </c>
+      <c r="C60" t="s">
+        <v>19</v>
+      </c>
+      <c r="D60" t="b">
+        <v>1</v>
+      </c>
+      <c r="E60" t="b">
+        <v>0</v>
+      </c>
+      <c r="F60" t="b">
+        <v>0</v>
+      </c>
+      <c r="G60" t="b">
+        <v>0</v>
+      </c>
+      <c r="H60" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated peeps accounting and saved carrocket psd
</commit_message>
<xml_diff>
--- a/Garden App/Peeps Accounting.xlsx
+++ b/Garden App/Peeps Accounting.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bi-lea\Source\Repos\OpenSource\codegarden-2020-group-image-another-dimension\Garden App\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lars-\source\repos\open source\cg2020-group-picture-another-dimension\Garden App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{008BE434-FC7A-4B74-A6C8-6207949516FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC3EC96-DF5B-44C2-8F44-75CF707F3B36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{8684E3AA-EC06-48A7-BFAE-7CCFBD7EFAE6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8684E3AA-EC06-48A7-BFAE-7CCFBD7EFAE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="80">
   <si>
     <t>Name</t>
   </si>
@@ -270,6 +270,9 @@
   </si>
   <si>
     <t>Nick W.</t>
+  </si>
+  <si>
+    <t>Emma G</t>
   </si>
 </sst>
 </file>
@@ -325,8 +328,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{91054EBE-4800-4CD4-9A7C-F2794396E173}" name="Table1" displayName="Table1" ref="A1:I60" totalsRowShown="0">
-  <autoFilter ref="A1:I60" xr:uid="{1D6FD3FD-DD4E-4958-8C16-1C6223DC65F8}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{91054EBE-4800-4CD4-9A7C-F2794396E173}" name="Table1" displayName="Table1" ref="A1:I61" totalsRowShown="0">
+  <autoFilter ref="A1:I61" xr:uid="{1D6FD3FD-DD4E-4958-8C16-1C6223DC65F8}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{F70AE9DF-F9FB-486D-8564-B7D56E3818A4}" name="Name"/>
     <tableColumn id="9" xr3:uid="{7799C646-F115-4391-AD0A-F12801AF397D}" name="No. of peeps"/>
@@ -639,10 +642,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D97C0BEB-74C8-4333-889B-395318AF70D1}">
-  <dimension ref="A1:I60"/>
+  <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2157,7 +2160,7 @@
         <v>1</v>
       </c>
       <c r="E57" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F57" t="b">
         <v>0</v>
@@ -2183,7 +2186,7 @@
         <v>1</v>
       </c>
       <c r="E58" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F58" t="b">
         <v>0</v>
@@ -2244,6 +2247,32 @@
         <v>0</v>
       </c>
       <c r="H60" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>79</v>
+      </c>
+      <c r="B61">
+        <v>1</v>
+      </c>
+      <c r="C61" t="s">
+        <v>23</v>
+      </c>
+      <c r="D61" t="b">
+        <v>1</v>
+      </c>
+      <c r="E61" t="b">
+        <v>0</v>
+      </c>
+      <c r="F61" t="b">
+        <v>0</v>
+      </c>
+      <c r="G61" t="b">
+        <v>0</v>
+      </c>
+      <c r="H61" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>